<commit_message>
Se crea robot para crear OTs
</commit_message>
<xml_diff>
--- a/BUSCAR EN MAXIMO CARGAS/data/datos.xlsx
+++ b/BUSCAR EN MAXIMO CARGAS/data/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eruhern\Documents\UiPath\BUSCAR EN MAXIMO CARGAS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC1AC3E-CF38-4A74-947E-15075E79A111}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6E2EAE-5EBA-4B5B-BB27-F19DA2BFF13C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="14980" activeTab="1" xr2:uid="{8B51D6BE-9F50-4663-859D-D701AB2BE83D}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,7 +549,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>